<commit_message>
added filepath for database
</commit_message>
<xml_diff>
--- a/Data/Database.xlsx
+++ b/Data/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Dropbox\01_Master_Thesis\06_KBOB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Dropbox\01_Master_Thesis\05_Python\App\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B134CBA-8484-4F85-B682-F2D73F89F082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11E822D-ED28-4FED-BFA4-60C69A15A0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1815" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1815" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="414">
   <si>
     <t>Vorbereitungsarbeiten</t>
   </si>
@@ -1585,6 +1585,9 @@
   </si>
   <si>
     <t>Interior door, wood</t>
+  </si>
+  <si>
+    <t>CHANGE  DATA  TO BE CALCULATED</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1728,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1782,24 +1785,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCBF1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1812,7 +1797,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="8"/>
       </patternFill>
     </fill>
@@ -1931,7 +1916,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2253,22 +2238,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2329,10 +2299,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2388,57 +2358,77 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="14" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="11" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="12" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3463,10 +3453,10 @@
       <c r="F1" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="110" t="s">
         <v>350</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="110" t="s">
         <v>394</v>
       </c>
     </row>
@@ -3498,7 +3488,7 @@
       <c r="D3" s="28">
         <v>911</v>
       </c>
-      <c r="E3" s="157">
+      <c r="E3" s="152">
         <v>850</v>
       </c>
       <c r="F3" s="72">
@@ -3521,7 +3511,7 @@
       <c r="D4" s="28">
         <v>872</v>
       </c>
-      <c r="E4" s="157">
+      <c r="E4" s="152">
         <v>810</v>
       </c>
       <c r="F4" s="72">
@@ -5410,369 +5400,369 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="116">
+    <row r="88" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="111">
         <v>5.0039999999999996</v>
       </c>
-      <c r="B88" s="117" t="s">
+      <c r="B88" s="112" t="s">
         <v>411</v>
       </c>
-      <c r="C88" s="118" t="s">
+      <c r="C88" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D88" s="161">
+      <c r="D88" s="156">
         <v>133</v>
       </c>
-      <c r="E88" s="162">
+      <c r="E88" s="157">
         <v>118</v>
       </c>
-      <c r="F88" s="163">
+      <c r="F88" s="158">
         <v>14.9</v>
       </c>
       <c r="G88">
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="122">
+    <row r="89" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="117">
         <v>5.0040100000000001</v>
       </c>
-      <c r="B89" s="117" t="s">
+      <c r="B89" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="C89" s="123" t="s">
+      <c r="C89" s="118" t="s">
         <v>287</v>
       </c>
-      <c r="D89" s="124">
+      <c r="D89" s="119">
         <v>203</v>
       </c>
-      <c r="E89" s="125">
+      <c r="E89" s="120">
         <v>182</v>
       </c>
-      <c r="F89" s="126">
+      <c r="F89" s="121">
         <v>21.4</v>
       </c>
       <c r="G89">
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="116">
+    <row r="90" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="111">
         <v>5.0049999999999999</v>
       </c>
-      <c r="B90" s="117" t="s">
+      <c r="B90" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="C90" s="118" t="s">
+      <c r="C90" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D90" s="127">
+      <c r="D90" s="122">
         <v>128</v>
       </c>
-      <c r="E90" s="128">
+      <c r="E90" s="123">
         <v>109</v>
       </c>
-      <c r="F90" s="129">
+      <c r="F90" s="124">
         <v>19.600000000000001</v>
       </c>
       <c r="G90">
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="116">
+    <row r="91" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="111">
         <v>5.0060000000000002</v>
       </c>
-      <c r="B91" s="117" t="s">
+      <c r="B91" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="C91" s="118" t="s">
+      <c r="C91" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D91" s="127">
+      <c r="D91" s="122">
         <v>217</v>
       </c>
-      <c r="E91" s="128">
+      <c r="E91" s="123">
         <v>191</v>
       </c>
-      <c r="F91" s="129">
+      <c r="F91" s="124">
         <v>25.7</v>
       </c>
       <c r="G91">
         <v>0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="116">
+    <row r="92" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="111">
         <v>5.0069999999999997</v>
       </c>
-      <c r="B92" s="117" t="s">
+      <c r="B92" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="C92" s="118" t="s">
+      <c r="C92" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D92" s="119">
+      <c r="D92" s="114">
         <v>285</v>
       </c>
-      <c r="E92" s="120">
+      <c r="E92" s="115">
         <v>228</v>
       </c>
-      <c r="F92" s="120">
+      <c r="F92" s="115">
         <v>57.2</v>
       </c>
       <c r="G92">
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="116">
+    <row r="93" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="111">
         <v>5.0010000000000003</v>
       </c>
-      <c r="B93" s="117" t="s">
+      <c r="B93" s="112" t="s">
         <v>96</v>
       </c>
-      <c r="C93" s="118" t="s">
+      <c r="C93" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D93" s="130">
+      <c r="D93" s="125">
         <v>43.7</v>
       </c>
-      <c r="E93" s="131">
+      <c r="E93" s="126">
         <v>39.799999999999997</v>
       </c>
-      <c r="F93" s="126">
+      <c r="F93" s="121">
         <v>3.88</v>
       </c>
       <c r="G93">
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="132">
+    <row r="94" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="127">
         <v>5.0090000000000003</v>
       </c>
-      <c r="B94" s="117" t="s">
+      <c r="B94" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="133" t="s">
+      <c r="C94" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D94" s="130">
+      <c r="D94" s="125">
         <v>47.9</v>
       </c>
-      <c r="E94" s="131">
+      <c r="E94" s="126">
         <v>44.9</v>
       </c>
-      <c r="F94" s="126">
+      <c r="F94" s="121">
         <v>2.98</v>
       </c>
       <c r="G94">
         <v>0.05</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="132">
+    <row r="95" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="127">
         <v>5.01</v>
       </c>
-      <c r="B95" s="117" t="s">
+      <c r="B95" s="112" t="s">
         <v>98</v>
       </c>
-      <c r="C95" s="133" t="s">
+      <c r="C95" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D95" s="130">
+      <c r="D95" s="125">
         <v>51.1</v>
       </c>
-      <c r="E95" s="131">
+      <c r="E95" s="126">
         <v>47.2</v>
       </c>
-      <c r="F95" s="126">
+      <c r="F95" s="121">
         <v>3.88</v>
       </c>
       <c r="G95">
         <v>0.05</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="116">
+    <row r="96" spans="1:7" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="111">
         <v>5.0019999999999998</v>
       </c>
-      <c r="B96" s="117" t="s">
+      <c r="B96" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="C96" s="118" t="s">
+      <c r="C96" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D96" s="130">
+      <c r="D96" s="125">
         <v>78.2</v>
       </c>
-      <c r="E96" s="131">
+      <c r="E96" s="126">
         <v>71.099999999999994</v>
       </c>
-      <c r="F96" s="126">
+      <c r="F96" s="121">
         <v>7.16</v>
       </c>
       <c r="G96">
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="132">
+    <row r="97" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="127">
         <v>5.0110000000000001</v>
       </c>
-      <c r="B97" s="117" t="s">
+      <c r="B97" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="C97" s="133" t="s">
+      <c r="C97" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D97" s="130">
+      <c r="D97" s="125">
         <v>85.6</v>
       </c>
-      <c r="E97" s="131">
+      <c r="E97" s="126">
         <v>78.400000000000006</v>
       </c>
-      <c r="F97" s="126">
+      <c r="F97" s="121">
         <v>7.16</v>
       </c>
       <c r="G97">
         <v>0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="116">
+    <row r="98" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="111">
         <v>5.0030000000000001</v>
       </c>
-      <c r="B98" s="117" t="s">
+      <c r="B98" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="C98" s="118" t="s">
+      <c r="C98" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="D98" s="130">
+      <c r="D98" s="125">
         <v>77.3</v>
       </c>
-      <c r="E98" s="131">
+      <c r="E98" s="126">
         <v>72.099999999999994</v>
       </c>
-      <c r="F98" s="126">
+      <c r="F98" s="121">
         <v>5.25</v>
       </c>
       <c r="G98">
         <v>0.05</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="132">
+    <row r="99" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="127">
         <v>5.0119999999999996</v>
       </c>
-      <c r="B99" s="117" t="s">
+      <c r="B99" s="112" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="133" t="s">
+      <c r="C99" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D99" s="130">
+      <c r="D99" s="125">
         <v>66.8</v>
       </c>
-      <c r="E99" s="131">
+      <c r="E99" s="126">
         <v>60.7</v>
       </c>
-      <c r="F99" s="126">
+      <c r="F99" s="121">
         <v>6.16</v>
       </c>
       <c r="G99">
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="132">
+    <row r="100" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="127">
         <v>5.0129999999999999</v>
       </c>
-      <c r="B100" s="117" t="s">
+      <c r="B100" s="112" t="s">
         <v>103</v>
       </c>
-      <c r="C100" s="133" t="s">
+      <c r="C100" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D100" s="130">
+      <c r="D100" s="125">
         <v>81.599999999999994</v>
       </c>
-      <c r="E100" s="131">
+      <c r="E100" s="126">
         <v>75.400000000000006</v>
       </c>
-      <c r="F100" s="126">
+      <c r="F100" s="121">
         <v>6.16</v>
       </c>
       <c r="G100">
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="132">
+    <row r="101" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="127">
         <v>5.0140000000000002</v>
       </c>
-      <c r="B101" s="117" t="s">
+      <c r="B101" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="C101" s="133" t="s">
+      <c r="C101" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D101" s="130">
+      <c r="D101" s="125">
         <v>88.9</v>
       </c>
-      <c r="E101" s="131">
+      <c r="E101" s="126">
         <v>82.7</v>
       </c>
-      <c r="F101" s="126">
+      <c r="F101" s="121">
         <v>6.16</v>
       </c>
       <c r="G101">
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="132">
+    <row r="102" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="127">
         <v>5.0149999999999997</v>
       </c>
-      <c r="B102" s="117" t="s">
+      <c r="B102" s="112" t="s">
         <v>105</v>
       </c>
-      <c r="C102" s="133" t="s">
+      <c r="C102" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D102" s="130">
+      <c r="D102" s="125">
         <v>101</v>
       </c>
-      <c r="E102" s="131">
+      <c r="E102" s="126">
         <v>92</v>
       </c>
-      <c r="F102" s="126">
+      <c r="F102" s="121">
         <v>9.4499999999999993</v>
       </c>
       <c r="G102">
         <v>0.05</v>
       </c>
-      <c r="H102" s="155"/>
-    </row>
-    <row r="103" spans="1:8" s="121" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="132">
+      <c r="H102" s="150"/>
+    </row>
+    <row r="103" spans="1:8" s="116" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="127">
         <v>5.016</v>
       </c>
-      <c r="B103" s="117" t="s">
+      <c r="B103" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="C103" s="133" t="s">
+      <c r="C103" s="128" t="s">
         <v>287</v>
       </c>
-      <c r="D103" s="130">
+      <c r="D103" s="125">
         <v>110</v>
       </c>
-      <c r="E103" s="131">
+      <c r="E103" s="126">
         <v>100</v>
       </c>
-      <c r="F103" s="126">
+      <c r="F103" s="121">
         <v>9.4499999999999993</v>
       </c>
       <c r="G103">
@@ -5990,13 +5980,13 @@
       <c r="C113" s="16">
         <v>7850</v>
       </c>
-      <c r="D113" s="158">
+      <c r="D113" s="153">
         <v>1.52</v>
       </c>
-      <c r="E113" s="159">
+      <c r="E113" s="154">
         <v>1.5</v>
       </c>
-      <c r="F113" s="160">
+      <c r="F113" s="155">
         <v>1.24E-2</v>
       </c>
       <c r="G113">
@@ -8829,13 +8819,13 @@
       <c r="C238" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="D238" s="164">
+      <c r="D238" s="159">
         <v>32.4</v>
       </c>
-      <c r="E238" s="165">
+      <c r="E238" s="160">
         <v>27</v>
       </c>
-      <c r="F238" s="166">
+      <c r="F238" s="161">
         <v>5.4</v>
       </c>
       <c r="G238">
@@ -10555,7 +10545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED689CC4-0898-49F8-8BE3-C6C7C16515AA}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -10574,311 +10564,311 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+    <row r="2" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="129" t="s">
         <v>351</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="130" t="s">
         <v>352</v>
       </c>
-      <c r="C2" s="136" t="s">
+      <c r="C2" s="131" t="s">
         <v>353</v>
       </c>
-      <c r="D2" s="136" t="s">
+      <c r="D2" s="131" t="s">
         <v>353</v>
       </c>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-    </row>
-    <row r="3" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+    </row>
+    <row r="3" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="134" t="s">
         <v>354</v>
       </c>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="135" t="s">
         <v>355</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="136" t="s">
         <v>356</v>
       </c>
-      <c r="D3" s="142">
+      <c r="D3" s="137">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E3" s="137"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-    </row>
-    <row r="4" spans="1:7" s="148" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="144" t="s">
+      <c r="E3" s="132"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+    </row>
+    <row r="4" spans="1:7" s="143" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="139" t="s">
         <v>357</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="135" t="s">
         <v>358</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="140" t="s">
         <v>359</v>
       </c>
-      <c r="D4" s="142">
+      <c r="D4" s="137">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E4" s="146"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-    </row>
-    <row r="5" spans="1:7" s="148" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="144" t="s">
+      <c r="E4" s="141"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+    </row>
+    <row r="5" spans="1:7" s="143" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="139" t="s">
         <v>360</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="135" t="s">
         <v>361</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="140" t="s">
         <v>359</v>
       </c>
-      <c r="D5" s="142">
+      <c r="D5" s="137">
         <v>0.40100000000000002</v>
       </c>
-      <c r="E5" s="146"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
-    </row>
-    <row r="6" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149" t="s">
+      <c r="E5" s="141"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+    </row>
+    <row r="6" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="144" t="s">
         <v>362</v>
       </c>
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="135" t="s">
         <v>363</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="C6" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D6" s="150">
+      <c r="D6" s="145">
         <v>4.7199999999999999E-2</v>
       </c>
-      <c r="E6" s="137"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-    </row>
-    <row r="7" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149" t="s">
+      <c r="E6" s="132"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
+    </row>
+    <row r="7" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="144" t="s">
         <v>365</v>
       </c>
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="135" t="s">
         <v>366</v>
       </c>
-      <c r="C7" s="141" t="s">
+      <c r="C7" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D7" s="152">
+      <c r="D7" s="147">
         <v>1.17</v>
       </c>
-      <c r="E7" s="137"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-    </row>
-    <row r="8" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149" t="s">
+      <c r="E7" s="132"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+    </row>
+    <row r="8" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="144" t="s">
         <v>367</v>
       </c>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="135" t="s">
         <v>368</v>
       </c>
-      <c r="C8" s="141" t="s">
+      <c r="C8" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D8" s="152">
+      <c r="D8" s="147">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E8" s="137"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-    </row>
-    <row r="9" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="149" t="s">
+      <c r="E8" s="132"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+    </row>
+    <row r="9" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="144" t="s">
         <v>369</v>
       </c>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="135" t="s">
         <v>370</v>
       </c>
-      <c r="C9" s="141" t="s">
+      <c r="C9" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="152">
+      <c r="D9" s="147">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-    </row>
-    <row r="10" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149" t="s">
+      <c r="E9" s="132"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+    </row>
+    <row r="10" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="144" t="s">
         <v>371</v>
       </c>
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="148" t="s">
         <v>372</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D10" s="150">
+      <c r="D10" s="145">
         <v>1.35E-2</v>
       </c>
-      <c r="E10" s="137"/>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-    </row>
-    <row r="11" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149" t="s">
+      <c r="E10" s="132"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+    </row>
+    <row r="11" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="144" t="s">
         <v>373</v>
       </c>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="135" t="s">
         <v>374</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C11" s="136" t="s">
         <v>375</v>
       </c>
-      <c r="D11" s="151">
+      <c r="D11" s="146">
         <v>100</v>
       </c>
-      <c r="E11" s="137"/>
-      <c r="F11" s="143"/>
-      <c r="G11" s="143"/>
-    </row>
-    <row r="12" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149" t="s">
+      <c r="E11" s="132"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
+    </row>
+    <row r="12" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="144" t="s">
         <v>376</v>
       </c>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="135" t="s">
         <v>377</v>
       </c>
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D12" s="150">
+      <c r="D12" s="145">
         <v>1.09E-2</v>
       </c>
-      <c r="E12" s="137"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="143"/>
-    </row>
-    <row r="13" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="149" t="s">
+      <c r="E12" s="132"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+    </row>
+    <row r="13" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="144" t="s">
         <v>378</v>
       </c>
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="148" t="s">
         <v>379</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="C13" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D13" s="154">
+      <c r="D13" s="149">
         <v>5.7299999999999999E-3</v>
       </c>
-      <c r="E13" s="137"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-    </row>
-    <row r="14" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="149" t="s">
+      <c r="E13" s="132"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+    </row>
+    <row r="14" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="144" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="135" t="s">
         <v>381</v>
       </c>
-      <c r="C14" s="141" t="s">
+      <c r="C14" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D14" s="152">
+      <c r="D14" s="147">
         <v>1.52</v>
       </c>
-      <c r="E14" s="137"/>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-    </row>
-    <row r="15" spans="1:7" s="148" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="144" t="s">
+      <c r="E14" s="132"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+    </row>
+    <row r="15" spans="1:7" s="143" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="139" t="s">
         <v>382</v>
       </c>
-      <c r="B15" s="140" t="s">
+      <c r="B15" s="135" t="s">
         <v>383</v>
       </c>
-      <c r="C15" s="145" t="s">
+      <c r="C15" s="140" t="s">
         <v>364</v>
       </c>
-      <c r="D15" s="142">
+      <c r="D15" s="137">
         <v>0.13500000000000001</v>
       </c>
-      <c r="E15" s="146"/>
-      <c r="F15" s="147"/>
-      <c r="G15" s="147"/>
-    </row>
-    <row r="16" spans="1:7" s="148" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="144" t="s">
+      <c r="E15" s="141"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+    </row>
+    <row r="16" spans="1:7" s="143" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="139" t="s">
         <v>384</v>
       </c>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="135" t="s">
         <v>385</v>
       </c>
-      <c r="C16" s="145" t="s">
+      <c r="C16" s="140" t="s">
         <v>364</v>
       </c>
-      <c r="D16" s="142">
+      <c r="D16" s="137">
         <v>0.51800000000000002</v>
       </c>
-      <c r="E16" s="146"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
-    </row>
-    <row r="17" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="149" t="s">
+      <c r="E16" s="141"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="142"/>
+    </row>
+    <row r="17" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="144" t="s">
         <v>386</v>
       </c>
-      <c r="B17" s="140" t="s">
+      <c r="B17" s="135" t="s">
         <v>387</v>
       </c>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D17" s="142">
+      <c r="D17" s="137">
         <v>0.218</v>
       </c>
-      <c r="E17" s="137"/>
-      <c r="F17" s="143"/>
-      <c r="G17" s="143"/>
-    </row>
-    <row r="18" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="149" t="s">
+      <c r="E17" s="132"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+    </row>
+    <row r="18" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="144" t="s">
         <v>388</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="135" t="s">
         <v>389</v>
       </c>
-      <c r="C18" s="141" t="s">
+      <c r="C18" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D18" s="142">
+      <c r="D18" s="137">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E18" s="137"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-    </row>
-    <row r="19" spans="1:7" s="138" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="149" t="s">
+      <c r="E18" s="132"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+    </row>
+    <row r="19" spans="1:7" s="133" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="144" t="s">
         <v>390</v>
       </c>
-      <c r="B19" s="140" t="s">
+      <c r="B19" s="135" t="s">
         <v>391</v>
       </c>
-      <c r="C19" s="141" t="s">
+      <c r="C19" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D19" s="142">
+      <c r="D19" s="137">
         <v>0.11</v>
       </c>
-      <c r="E19" s="137"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="138"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D19">
@@ -10910,64 +10900,64 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G194" sqref="G194"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="50.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="170" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="169" customWidth="1"/>
     <col min="5" max="5" width="18.54296875" style="90" customWidth="1"/>
     <col min="6" max="6" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="52" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:16" s="175" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A1" s="170" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="171" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="172" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="171" t="s">
+      <c r="D1" s="173" t="s">
         <v>406</v>
       </c>
-      <c r="E1" s="172" t="s">
+      <c r="E1" s="174" t="s">
         <v>395</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="171" t="s">
         <v>396</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="171" t="s">
         <v>405</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="171" t="s">
         <v>397</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="171" t="s">
         <v>398</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="171" t="s">
         <v>399</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="K1" s="173" t="s">
         <v>401</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="173" t="s">
         <v>403</v>
       </c>
-      <c r="M1" s="114" t="s">
+      <c r="M1" s="173" t="s">
         <v>400</v>
       </c>
-      <c r="N1" s="114" t="s">
+      <c r="N1" s="173" t="s">
         <v>402</v>
       </c>
-      <c r="O1" s="114" t="s">
+      <c r="O1" s="173" t="s">
         <v>404</v>
       </c>
-      <c r="P1" s="114"/>
+      <c r="P1" s="173"/>
     </row>
     <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
@@ -10990,10 +10980,10 @@
       <c r="C3" s="14">
         <v>2150</v>
       </c>
-      <c r="D3" s="170">
-        <v>0</v>
-      </c>
-      <c r="E3" s="173">
+      <c r="D3" s="169">
+        <v>0</v>
+      </c>
+      <c r="E3" s="166">
         <v>0.9</v>
       </c>
       <c r="F3">
@@ -11028,51 +11018,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="167">
+    <row r="4" spans="1:16" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="162">
         <v>1.002</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="169">
+      <c r="C4" s="164">
         <v>2300</v>
       </c>
-      <c r="D4" s="170">
-        <v>0</v>
-      </c>
-      <c r="E4" s="174">
+      <c r="D4" s="169">
+        <v>0</v>
+      </c>
+      <c r="E4" s="167">
         <v>0.85</v>
       </c>
-      <c r="F4" s="170">
+      <c r="F4" s="165">
         <v>0.15</v>
       </c>
-      <c r="G4" s="170">
-        <v>0</v>
-      </c>
-      <c r="H4" s="170">
-        <v>1</v>
-      </c>
-      <c r="I4" s="170">
-        <v>0</v>
-      </c>
-      <c r="J4" s="170">
-        <v>0</v>
-      </c>
-      <c r="K4" s="170">
-        <v>1</v>
-      </c>
-      <c r="L4" s="170">
-        <v>1</v>
-      </c>
-      <c r="M4" s="170">
-        <v>0</v>
-      </c>
-      <c r="N4" s="170">
+      <c r="G4" s="165">
+        <v>0</v>
+      </c>
+      <c r="H4" s="165">
+        <v>1</v>
+      </c>
+      <c r="I4" s="165">
+        <v>0</v>
+      </c>
+      <c r="J4" s="165">
+        <v>0</v>
+      </c>
+      <c r="K4" s="165">
+        <v>1</v>
+      </c>
+      <c r="L4" s="165">
+        <v>1</v>
+      </c>
+      <c r="M4" s="165">
+        <v>0</v>
+      </c>
+      <c r="N4" s="165">
         <f t="shared" ref="N4:N67" si="0">E4</f>
         <v>0.85</v>
       </c>
-      <c r="O4" s="170">
+      <c r="O4" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -11086,7 +11076,7 @@
       <c r="C5" s="14">
         <v>2350</v>
       </c>
-      <c r="D5" s="170">
+      <c r="D5" s="169">
         <v>0</v>
       </c>
       <c r="E5" s="90">
@@ -11134,7 +11124,7 @@
       <c r="C6" s="14">
         <v>2325</v>
       </c>
-      <c r="D6" s="170">
+      <c r="D6" s="169">
         <v>0</v>
       </c>
       <c r="E6" s="90">
@@ -11182,7 +11172,7 @@
       <c r="C7" s="14">
         <v>2770</v>
       </c>
-      <c r="D7" s="170">
+      <c r="D7" s="169">
         <v>0.5</v>
       </c>
       <c r="E7" s="90">
@@ -11230,7 +11220,7 @@
       <c r="C8" s="14">
         <v>2500</v>
       </c>
-      <c r="D8" s="170">
+      <c r="D8" s="169">
         <v>0.5</v>
       </c>
       <c r="E8" s="90">
@@ -11278,7 +11268,7 @@
       <c r="C9" s="14">
         <v>600</v>
       </c>
-      <c r="D9" s="170">
+      <c r="D9" s="169">
         <v>0</v>
       </c>
       <c r="E9" s="90">
@@ -11326,7 +11316,7 @@
       <c r="C10" s="15">
         <v>600</v>
       </c>
-      <c r="D10" s="170">
+      <c r="D10" s="169">
         <v>0</v>
       </c>
       <c r="E10" s="90">
@@ -11401,7 +11391,7 @@
       <c r="C12" s="14">
         <v>900</v>
       </c>
-      <c r="D12" s="170">
+      <c r="D12" s="169">
         <v>0</v>
       </c>
       <c r="E12" s="90">
@@ -11439,51 +11429,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="167">
+    <row r="13" spans="1:16" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="162">
         <v>2.0019999999999998</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="169">
+      <c r="C13" s="164">
         <v>1400</v>
       </c>
-      <c r="D13" s="170">
-        <v>0</v>
-      </c>
-      <c r="E13" s="174">
+      <c r="D13" s="169">
+        <v>0</v>
+      </c>
+      <c r="E13" s="167">
         <v>0.8</v>
       </c>
-      <c r="F13" s="170">
+      <c r="F13" s="165">
         <v>0.2</v>
       </c>
-      <c r="G13" s="170">
-        <v>0</v>
-      </c>
-      <c r="H13" s="170">
-        <v>1</v>
-      </c>
-      <c r="I13" s="170">
-        <v>0</v>
-      </c>
-      <c r="J13" s="170">
-        <v>0</v>
-      </c>
-      <c r="K13" s="170">
-        <v>1</v>
-      </c>
-      <c r="L13" s="170">
-        <v>1</v>
-      </c>
-      <c r="M13" s="170">
-        <v>0</v>
-      </c>
-      <c r="N13" s="170">
+      <c r="G13" s="165">
+        <v>0</v>
+      </c>
+      <c r="H13" s="165">
+        <v>1</v>
+      </c>
+      <c r="I13" s="165">
+        <v>0</v>
+      </c>
+      <c r="J13" s="165">
+        <v>0</v>
+      </c>
+      <c r="K13" s="165">
+        <v>1</v>
+      </c>
+      <c r="L13" s="165">
+        <v>1</v>
+      </c>
+      <c r="M13" s="165">
+        <v>0</v>
+      </c>
+      <c r="N13" s="165">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="O13" s="170">
+      <c r="O13" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -11497,7 +11487,7 @@
       <c r="C14" s="14">
         <v>1400</v>
       </c>
-      <c r="D14" s="170">
+      <c r="D14" s="169">
         <v>0</v>
       </c>
       <c r="E14" s="90">
@@ -11545,7 +11535,7 @@
       <c r="C15" s="14">
         <v>700</v>
       </c>
-      <c r="D15" s="170">
+      <c r="D15" s="169">
         <v>0</v>
       </c>
       <c r="E15" s="90">
@@ -11593,7 +11583,7 @@
       <c r="C16" s="14">
         <v>1200</v>
       </c>
-      <c r="D16" s="170">
+      <c r="D16" s="169">
         <v>0</v>
       </c>
       <c r="E16" s="90">
@@ -11641,7 +11631,7 @@
       <c r="C17" s="15">
         <v>1200</v>
       </c>
-      <c r="D17" s="170">
+      <c r="D17" s="169">
         <v>0</v>
       </c>
       <c r="E17" s="90">
@@ -11689,7 +11679,7 @@
       <c r="C18" s="14">
         <v>500</v>
       </c>
-      <c r="D18" s="170">
+      <c r="D18" s="169">
         <v>0</v>
       </c>
       <c r="E18" s="90">
@@ -11737,7 +11727,7 @@
       <c r="C19" s="14">
         <v>1700</v>
       </c>
-      <c r="D19" s="170">
+      <c r="D19" s="169">
         <v>0</v>
       </c>
       <c r="E19" s="90">
@@ -11824,7 +11814,7 @@
       <c r="C21" s="14">
         <v>2300</v>
       </c>
-      <c r="D21" s="170">
+      <c r="D21" s="169">
         <v>0</v>
       </c>
       <c r="E21" s="90">
@@ -11872,7 +11862,7 @@
       <c r="C22" s="14">
         <v>1800</v>
       </c>
-      <c r="D22" s="170">
+      <c r="D22" s="169">
         <v>0</v>
       </c>
       <c r="E22" s="90">
@@ -11921,7 +11911,7 @@
       <c r="C23" s="14">
         <v>1800</v>
       </c>
-      <c r="D23" s="170">
+      <c r="D23" s="169">
         <v>0</v>
       </c>
       <c r="E23" s="90">
@@ -11970,7 +11960,7 @@
       <c r="C24" s="15">
         <v>1800</v>
       </c>
-      <c r="D24" s="170">
+      <c r="D24" s="169">
         <v>0</v>
       </c>
       <c r="E24" s="90">
@@ -12019,7 +12009,7 @@
       <c r="C25" s="14">
         <v>2500</v>
       </c>
-      <c r="D25" s="170">
+      <c r="D25" s="169">
         <v>0</v>
       </c>
       <c r="E25" s="90">
@@ -12068,7 +12058,7 @@
       <c r="C26" s="14">
         <v>2500</v>
       </c>
-      <c r="D26" s="170">
+      <c r="D26" s="169">
         <v>0</v>
       </c>
       <c r="E26" s="90">
@@ -12117,7 +12107,7 @@
       <c r="C27" s="14">
         <v>1200</v>
       </c>
-      <c r="D27" s="170">
+      <c r="D27" s="169">
         <v>0</v>
       </c>
       <c r="E27" s="90">
@@ -12166,7 +12156,7 @@
       <c r="C28" s="14">
         <v>850</v>
       </c>
-      <c r="D28" s="170">
+      <c r="D28" s="169">
         <v>0</v>
       </c>
       <c r="E28" s="90">
@@ -12215,7 +12205,7 @@
       <c r="C29" s="14">
         <v>1000</v>
       </c>
-      <c r="D29" s="170">
+      <c r="D29" s="169">
         <v>0</v>
       </c>
       <c r="E29" s="90">
@@ -12264,7 +12254,7 @@
       <c r="C30" s="14">
         <v>2500</v>
       </c>
-      <c r="D30" s="170">
+      <c r="D30" s="169">
         <v>0</v>
       </c>
       <c r="E30" s="90">
@@ -12313,7 +12303,7 @@
       <c r="C31" s="15">
         <v>2600</v>
       </c>
-      <c r="D31" s="170">
+      <c r="D31" s="169">
         <v>0</v>
       </c>
       <c r="E31" s="90">
@@ -12362,7 +12352,7 @@
       <c r="C32" s="14">
         <v>2600</v>
       </c>
-      <c r="D32" s="170">
+      <c r="D32" s="169">
         <v>0</v>
       </c>
       <c r="E32" s="90">
@@ -12411,7 +12401,7 @@
       <c r="C33" s="14">
         <v>2000</v>
       </c>
-      <c r="D33" s="170">
+      <c r="D33" s="169">
         <v>0</v>
       </c>
       <c r="E33" s="90">
@@ -12460,7 +12450,7 @@
       <c r="C34" s="14">
         <v>2000</v>
       </c>
-      <c r="D34" s="170">
+      <c r="D34" s="169">
         <v>0</v>
       </c>
       <c r="E34" s="90">
@@ -12509,7 +12499,7 @@
       <c r="C35" s="14">
         <v>2000</v>
       </c>
-      <c r="D35" s="170">
+      <c r="D35" s="169">
         <v>0</v>
       </c>
       <c r="E35" s="90">
@@ -12558,7 +12548,7 @@
       <c r="C36" s="14">
         <v>2000</v>
       </c>
-      <c r="D36" s="170">
+      <c r="D36" s="169">
         <v>0</v>
       </c>
       <c r="E36" s="90">
@@ -12607,7 +12597,7 @@
       <c r="C37" s="14">
         <v>2000</v>
       </c>
-      <c r="D37" s="170">
+      <c r="D37" s="169">
         <v>0</v>
       </c>
       <c r="E37" s="90">
@@ -12656,7 +12646,7 @@
       <c r="C38" s="15">
         <v>1700</v>
       </c>
-      <c r="D38" s="170">
+      <c r="D38" s="169">
         <v>0</v>
       </c>
       <c r="E38" s="90">
@@ -13275,7 +13265,7 @@
       <c r="C58" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D58" s="170">
+      <c r="D58" s="169">
         <v>0.25</v>
       </c>
       <c r="E58" s="90">
@@ -13324,7 +13314,7 @@
       <c r="C59" s="15">
         <v>7.1</v>
       </c>
-      <c r="D59" s="170">
+      <c r="D59" s="169">
         <v>0.5</v>
       </c>
       <c r="E59" s="90">
@@ -13373,7 +13363,7 @@
       <c r="C60" s="14">
         <v>11.6</v>
       </c>
-      <c r="D60" s="170">
+      <c r="D60" s="169">
         <v>0.25</v>
       </c>
       <c r="E60" s="90">
@@ -13422,7 +13412,7 @@
       <c r="C61" s="14">
         <v>78</v>
       </c>
-      <c r="D61" s="170">
+      <c r="D61" s="169">
         <v>0.25</v>
       </c>
       <c r="E61" s="90">
@@ -13471,7 +13461,7 @@
       <c r="C62" s="14">
         <v>2.4</v>
       </c>
-      <c r="D62" s="170">
+      <c r="D62" s="169">
         <v>0.25</v>
       </c>
       <c r="E62" s="90">
@@ -13510,52 +13500,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="175">
+    <row r="63" spans="1:15" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="168">
         <v>5.0039999999999996</v>
       </c>
-      <c r="B63" s="168" t="s">
+      <c r="B63" s="163" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="169" t="s">
+      <c r="C63" s="164" t="s">
         <v>287</v>
       </c>
-      <c r="D63" s="170">
+      <c r="D63" s="169">
         <v>0.25</v>
       </c>
-      <c r="E63" s="174">
+      <c r="E63" s="167">
         <v>0.98</v>
       </c>
-      <c r="F63" s="170">
+      <c r="F63" s="165">
         <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="G63" s="170">
-        <v>1</v>
-      </c>
-      <c r="H63" s="170">
-        <v>0</v>
-      </c>
-      <c r="I63" s="170">
-        <v>0</v>
-      </c>
-      <c r="J63" s="170">
-        <v>0</v>
-      </c>
-      <c r="K63" s="170">
-        <v>1</v>
-      </c>
-      <c r="L63" s="170">
-        <v>1</v>
-      </c>
-      <c r="M63" s="170">
-        <v>0</v>
-      </c>
-      <c r="N63" s="170">
+      <c r="G63" s="165">
+        <v>1</v>
+      </c>
+      <c r="H63" s="165">
+        <v>0</v>
+      </c>
+      <c r="I63" s="165">
+        <v>0</v>
+      </c>
+      <c r="J63" s="165">
+        <v>0</v>
+      </c>
+      <c r="K63" s="165">
+        <v>1</v>
+      </c>
+      <c r="L63" s="165">
+        <v>1</v>
+      </c>
+      <c r="M63" s="165">
+        <v>0</v>
+      </c>
+      <c r="N63" s="165">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
-      <c r="O63" s="170">
+      <c r="O63" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -13569,7 +13559,7 @@
       <c r="C64" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D64" s="170">
+      <c r="D64" s="169">
         <v>0.25</v>
       </c>
       <c r="E64" s="90">
@@ -13618,7 +13608,7 @@
       <c r="C65" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D65" s="170">
+      <c r="D65" s="169">
         <v>0.25</v>
       </c>
       <c r="E65" s="90">
@@ -13667,7 +13657,7 @@
       <c r="C66" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="D66" s="170">
+      <c r="D66" s="169">
         <v>0.25</v>
       </c>
       <c r="E66" s="90">
@@ -13716,7 +13706,7 @@
       <c r="C67" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D67" s="170">
+      <c r="D67" s="169">
         <v>0.25</v>
       </c>
       <c r="E67" s="90">
@@ -13765,7 +13755,7 @@
       <c r="C68" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D68" s="170">
+      <c r="D68" s="169">
         <v>0.25</v>
       </c>
       <c r="E68" s="90">
@@ -13814,7 +13804,7 @@
       <c r="C69" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D69" s="170">
+      <c r="D69" s="169">
         <v>0.25</v>
       </c>
       <c r="E69" s="90">
@@ -13863,7 +13853,7 @@
       <c r="C70" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D70" s="170">
+      <c r="D70" s="169">
         <v>0.25</v>
       </c>
       <c r="E70" s="90">
@@ -13912,7 +13902,7 @@
       <c r="C71" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D71" s="170">
+      <c r="D71" s="169">
         <v>0.25</v>
       </c>
       <c r="E71" s="90">
@@ -13961,7 +13951,7 @@
       <c r="C72" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D72" s="170">
+      <c r="D72" s="169">
         <v>0.25</v>
       </c>
       <c r="E72" s="90">
@@ -14010,7 +14000,7 @@
       <c r="C73" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="D73" s="170">
+      <c r="D73" s="169">
         <v>0.25</v>
       </c>
       <c r="E73" s="90">
@@ -14059,7 +14049,7 @@
       <c r="C74" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D74" s="170">
+      <c r="D74" s="169">
         <v>0.25</v>
       </c>
       <c r="E74" s="90">
@@ -14108,7 +14098,7 @@
       <c r="C75" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D75" s="170">
+      <c r="D75" s="169">
         <v>0.25</v>
       </c>
       <c r="E75" s="90">
@@ -14157,7 +14147,7 @@
       <c r="C76" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D76" s="170">
+      <c r="D76" s="169">
         <v>0.25</v>
       </c>
       <c r="E76" s="90">
@@ -14206,7 +14196,7 @@
       <c r="C77" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D77" s="170">
+      <c r="D77" s="169">
         <v>0.25</v>
       </c>
       <c r="E77" s="90">
@@ -14255,7 +14245,7 @@
       <c r="C78" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D78" s="170">
+      <c r="D78" s="169">
         <v>0.25</v>
       </c>
       <c r="E78" s="90">
@@ -14484,7 +14474,7 @@
       <c r="C85" s="14">
         <v>2690</v>
       </c>
-      <c r="D85" s="170">
+      <c r="D85" s="169">
         <v>0.75</v>
       </c>
       <c r="E85" s="90">
@@ -14533,7 +14523,7 @@
       <c r="C86" s="14">
         <v>2690</v>
       </c>
-      <c r="D86" s="170">
+      <c r="D86" s="169">
         <v>0.75</v>
       </c>
       <c r="E86" s="90">
@@ -14582,7 +14572,7 @@
       <c r="C87" s="15">
         <v>2690</v>
       </c>
-      <c r="D87" s="170">
+      <c r="D87" s="169">
         <v>0.75</v>
       </c>
       <c r="E87" s="90">
@@ -14621,52 +14611,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="167">
+    <row r="88" spans="1:15" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="162">
         <v>6.0030000000000001</v>
       </c>
-      <c r="B88" s="168" t="s">
+      <c r="B88" s="163" t="s">
         <v>117</v>
       </c>
-      <c r="C88" s="169">
+      <c r="C88" s="164">
         <v>7850</v>
       </c>
-      <c r="D88" s="170">
-        <v>0</v>
-      </c>
-      <c r="E88" s="174">
+      <c r="D88" s="169">
+        <v>0</v>
+      </c>
+      <c r="E88" s="167">
         <v>0.98</v>
       </c>
-      <c r="F88" s="170">
+      <c r="F88" s="165">
         <f t="shared" si="2"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="G88" s="170">
-        <v>0</v>
-      </c>
-      <c r="H88" s="170">
-        <v>1</v>
-      </c>
-      <c r="I88" s="170">
-        <v>0</v>
-      </c>
-      <c r="J88" s="170">
-        <v>0</v>
-      </c>
-      <c r="K88" s="170">
-        <v>1</v>
-      </c>
-      <c r="L88" s="170">
-        <v>1</v>
-      </c>
-      <c r="M88" s="170">
-        <v>0</v>
-      </c>
-      <c r="N88" s="170">
+      <c r="G88" s="165">
+        <v>0</v>
+      </c>
+      <c r="H88" s="165">
+        <v>1</v>
+      </c>
+      <c r="I88" s="165">
+        <v>0</v>
+      </c>
+      <c r="J88" s="165">
+        <v>0</v>
+      </c>
+      <c r="K88" s="165">
+        <v>1</v>
+      </c>
+      <c r="L88" s="165">
+        <v>1</v>
+      </c>
+      <c r="M88" s="165">
+        <v>0</v>
+      </c>
+      <c r="N88" s="165">
         <f t="shared" si="3"/>
         <v>0.98</v>
       </c>
-      <c r="O88" s="170">
+      <c r="O88" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -14680,7 +14670,7 @@
       <c r="C89" s="14">
         <v>11340</v>
       </c>
-      <c r="D89" s="170">
+      <c r="D89" s="169">
         <v>0.75</v>
       </c>
       <c r="E89" s="90">
@@ -14729,7 +14719,7 @@
       <c r="C90" s="14">
         <v>7900</v>
       </c>
-      <c r="D90" s="170">
+      <c r="D90" s="169">
         <v>0.75</v>
       </c>
       <c r="E90" s="90">
@@ -14778,7 +14768,7 @@
       <c r="C91" s="14">
         <v>7900</v>
       </c>
-      <c r="D91" s="170">
+      <c r="D91" s="169">
         <v>0.75</v>
       </c>
       <c r="E91" s="90">
@@ -14827,7 +14817,7 @@
       <c r="C92" s="14">
         <v>7700</v>
       </c>
-      <c r="D92" s="170">
+      <c r="D92" s="169">
         <v>0.75</v>
       </c>
       <c r="E92" s="90">
@@ -14876,7 +14866,7 @@
       <c r="C93" s="14">
         <v>7700</v>
       </c>
-      <c r="D93" s="170">
+      <c r="D93" s="169">
         <v>0.75</v>
       </c>
       <c r="E93" s="90">
@@ -14925,7 +14915,7 @@
       <c r="C94" s="15">
         <v>8900</v>
       </c>
-      <c r="D94" s="170">
+      <c r="D94" s="169">
         <v>0.75</v>
       </c>
       <c r="E94" s="90">
@@ -14974,7 +14964,7 @@
       <c r="C95" s="14">
         <v>8300</v>
       </c>
-      <c r="D95" s="170">
+      <c r="D95" s="169">
         <v>0.75</v>
       </c>
       <c r="E95" s="90">
@@ -15023,7 +15013,7 @@
       <c r="C96" s="14">
         <v>7850</v>
       </c>
-      <c r="D96" s="170">
+      <c r="D96" s="169">
         <v>0.75</v>
       </c>
       <c r="E96" s="90">
@@ -15072,7 +15062,7 @@
       <c r="C97" s="14">
         <v>7850</v>
       </c>
-      <c r="D97" s="170">
+      <c r="D97" s="169">
         <v>0.75</v>
       </c>
       <c r="E97" s="90">
@@ -15121,7 +15111,7 @@
       <c r="C98" s="14">
         <v>7850</v>
       </c>
-      <c r="D98" s="170">
+      <c r="D98" s="169">
         <v>0.75</v>
       </c>
       <c r="E98" s="90">
@@ -15170,7 +15160,7 @@
       <c r="C99" s="14">
         <v>7200</v>
       </c>
-      <c r="D99" s="170">
+      <c r="D99" s="169">
         <v>0.75</v>
       </c>
       <c r="E99" s="90">
@@ -15219,7 +15209,7 @@
       <c r="C100" s="105" t="s">
         <v>288</v>
       </c>
-      <c r="D100" s="170">
+      <c r="D100" s="169">
         <v>0</v>
       </c>
       <c r="J100">
@@ -15252,7 +15242,7 @@
       <c r="C101" s="15">
         <v>470</v>
       </c>
-      <c r="D101" s="170">
+      <c r="D101" s="169">
         <v>0.75</v>
       </c>
       <c r="E101" s="90">
@@ -15290,101 +15280,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:15" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="167">
+    <row r="102" spans="1:15" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="162">
         <v>7.0030000000000001</v>
       </c>
-      <c r="B102" s="168" t="s">
+      <c r="B102" s="163" t="s">
         <v>132</v>
       </c>
-      <c r="C102" s="169">
+      <c r="C102" s="164">
         <v>470</v>
       </c>
-      <c r="D102" s="170">
+      <c r="D102" s="169">
         <v>0.75</v>
       </c>
-      <c r="E102" s="174">
+      <c r="E102" s="167">
         <v>0.1</v>
       </c>
-      <c r="F102" s="170">
+      <c r="F102" s="165">
         <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
-      <c r="G102" s="170">
-        <v>1</v>
-      </c>
-      <c r="H102" s="170">
-        <v>0</v>
-      </c>
-      <c r="I102" s="170">
-        <v>0</v>
-      </c>
-      <c r="J102" s="170">
-        <v>0</v>
-      </c>
-      <c r="K102" s="170">
-        <v>1</v>
-      </c>
-      <c r="L102" s="170">
-        <v>1</v>
-      </c>
-      <c r="M102" s="170">
-        <v>0</v>
-      </c>
-      <c r="N102" s="170">
+      <c r="G102" s="165">
+        <v>1</v>
+      </c>
+      <c r="H102" s="165">
+        <v>0</v>
+      </c>
+      <c r="I102" s="165">
+        <v>0</v>
+      </c>
+      <c r="J102" s="165">
+        <v>0</v>
+      </c>
+      <c r="K102" s="165">
+        <v>1</v>
+      </c>
+      <c r="L102" s="165">
+        <v>1</v>
+      </c>
+      <c r="M102" s="165">
+        <v>0</v>
+      </c>
+      <c r="N102" s="165">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O102" s="170">
+      <c r="O102" s="165">
         <v>0.8</v>
       </c>
     </row>
-    <row r="103" spans="1:15" s="170" customFormat="1" ht="25" x14ac:dyDescent="0.35">
-      <c r="A103" s="167">
+    <row r="103" spans="1:15" s="165" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+      <c r="A103" s="162">
         <v>7.0030099999999997</v>
       </c>
-      <c r="B103" s="168" t="s">
+      <c r="B103" s="163" t="s">
         <v>133</v>
       </c>
-      <c r="C103" s="169">
+      <c r="C103" s="164">
         <v>470</v>
       </c>
-      <c r="D103" s="170">
+      <c r="D103" s="169">
         <v>0.75</v>
       </c>
-      <c r="E103" s="174">
+      <c r="E103" s="167">
         <v>0.1</v>
       </c>
-      <c r="F103" s="170">
+      <c r="F103" s="165">
         <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
-      <c r="G103" s="170">
-        <v>1</v>
-      </c>
-      <c r="H103" s="170">
-        <v>0</v>
-      </c>
-      <c r="I103" s="170">
-        <v>0</v>
-      </c>
-      <c r="J103" s="170">
-        <v>0</v>
-      </c>
-      <c r="K103" s="170">
-        <v>1</v>
-      </c>
-      <c r="L103" s="170">
-        <v>1</v>
-      </c>
-      <c r="M103" s="170">
-        <v>0</v>
-      </c>
-      <c r="N103" s="170">
+      <c r="G103" s="165">
+        <v>1</v>
+      </c>
+      <c r="H103" s="165">
+        <v>0</v>
+      </c>
+      <c r="I103" s="165">
+        <v>0</v>
+      </c>
+      <c r="J103" s="165">
+        <v>0</v>
+      </c>
+      <c r="K103" s="165">
+        <v>1</v>
+      </c>
+      <c r="L103" s="165">
+        <v>1</v>
+      </c>
+      <c r="M103" s="165">
+        <v>0</v>
+      </c>
+      <c r="N103" s="165">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O103" s="170">
+      <c r="O103" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -15398,7 +15388,7 @@
       <c r="C104" s="14">
         <v>470</v>
       </c>
-      <c r="D104" s="170">
+      <c r="D104" s="169">
         <v>0.75</v>
       </c>
       <c r="E104" s="90">
@@ -15447,7 +15437,7 @@
       <c r="C105" s="14">
         <v>470</v>
       </c>
-      <c r="D105" s="170">
+      <c r="D105" s="169">
         <v>0.75</v>
       </c>
       <c r="E105" s="90">
@@ -15496,7 +15486,7 @@
       <c r="C106" s="14">
         <v>955</v>
       </c>
-      <c r="D106" s="170">
+      <c r="D106" s="169">
         <v>0.75</v>
       </c>
       <c r="E106" s="90">
@@ -15545,7 +15535,7 @@
       <c r="C107" s="14">
         <v>400</v>
       </c>
-      <c r="D107" s="170">
+      <c r="D107" s="169">
         <v>0.75</v>
       </c>
       <c r="E107" s="90">
@@ -15594,7 +15584,7 @@
       <c r="C108" s="15">
         <v>675</v>
       </c>
-      <c r="D108" s="170">
+      <c r="D108" s="169">
         <v>0.75</v>
       </c>
       <c r="E108" s="90">
@@ -15643,7 +15633,7 @@
       <c r="C109" s="14">
         <v>675</v>
       </c>
-      <c r="D109" s="170">
+      <c r="D109" s="169">
         <v>0.75</v>
       </c>
       <c r="E109" s="90">
@@ -15692,7 +15682,7 @@
       <c r="C110" s="14">
         <v>675</v>
       </c>
-      <c r="D110" s="170">
+      <c r="D110" s="169">
         <v>0.75</v>
       </c>
       <c r="E110" s="90">
@@ -15741,7 +15731,7 @@
       <c r="C111" s="14">
         <v>675</v>
       </c>
-      <c r="D111" s="170">
+      <c r="D111" s="169">
         <v>0.75</v>
       </c>
       <c r="E111" s="90">
@@ -15790,7 +15780,7 @@
       <c r="C112" s="14">
         <v>705</v>
       </c>
-      <c r="D112" s="170">
+      <c r="D112" s="169">
         <v>0.75</v>
       </c>
       <c r="E112" s="90">
@@ -15839,7 +15829,7 @@
       <c r="C113" s="14">
         <v>705</v>
       </c>
-      <c r="D113" s="170">
+      <c r="D113" s="169">
         <v>0.75</v>
       </c>
       <c r="E113" s="90">
@@ -15888,7 +15878,7 @@
       <c r="C114" s="14">
         <v>465</v>
       </c>
-      <c r="D114" s="170">
+      <c r="D114" s="169">
         <v>0.75</v>
       </c>
       <c r="E114" s="90">
@@ -15937,7 +15927,7 @@
       <c r="C115" s="15">
         <v>465</v>
       </c>
-      <c r="D115" s="170">
+      <c r="D115" s="169">
         <v>0.75</v>
       </c>
       <c r="E115" s="90">
@@ -15986,7 +15976,7 @@
       <c r="C116" s="14">
         <v>420</v>
       </c>
-      <c r="D116" s="170">
+      <c r="D116" s="169">
         <v>0.75</v>
       </c>
       <c r="E116" s="90">
@@ -16035,7 +16025,7 @@
       <c r="C117" s="14">
         <v>485</v>
       </c>
-      <c r="D117" s="170">
+      <c r="D117" s="169">
         <v>0.75</v>
       </c>
       <c r="E117" s="90">
@@ -16084,7 +16074,7 @@
       <c r="C118" s="14">
         <v>485</v>
       </c>
-      <c r="D118" s="170">
+      <c r="D118" s="169">
         <v>0.75</v>
       </c>
       <c r="E118" s="90">
@@ -16133,7 +16123,7 @@
       <c r="C119" s="14">
         <v>485</v>
       </c>
-      <c r="D119" s="170">
+      <c r="D119" s="169">
         <v>0.75</v>
       </c>
       <c r="E119" s="90">
@@ -16182,7 +16172,7 @@
       <c r="C120" s="14">
         <v>485</v>
       </c>
-      <c r="D120" s="170">
+      <c r="D120" s="169">
         <v>0.75</v>
       </c>
       <c r="E120" s="90">
@@ -16231,7 +16221,7 @@
       <c r="C121" s="14">
         <v>685</v>
       </c>
-      <c r="D121" s="170">
+      <c r="D121" s="169">
         <v>0.75</v>
       </c>
       <c r="E121" s="90">
@@ -16280,7 +16270,7 @@
       <c r="C122" s="15">
         <v>605</v>
       </c>
-      <c r="D122" s="170">
+      <c r="D122" s="169">
         <v>0.75</v>
       </c>
       <c r="E122" s="90">
@@ -16329,7 +16319,7 @@
       <c r="C123" s="14">
         <v>640</v>
       </c>
-      <c r="D123" s="170">
+      <c r="D123" s="169">
         <v>0.75</v>
       </c>
       <c r="E123" s="90">
@@ -16378,7 +16368,7 @@
       <c r="C124" s="14">
         <v>640</v>
       </c>
-      <c r="D124" s="170">
+      <c r="D124" s="169">
         <v>0.75</v>
       </c>
       <c r="E124" s="90">
@@ -16427,7 +16417,7 @@
       <c r="C125" s="14">
         <v>640</v>
       </c>
-      <c r="D125" s="170">
+      <c r="D125" s="169">
         <v>0.75</v>
       </c>
       <c r="E125" s="90">
@@ -16476,7 +16466,7 @@
       <c r="C126" s="14">
         <v>500</v>
       </c>
-      <c r="D126" s="170">
+      <c r="D126" s="169">
         <v>0.75</v>
       </c>
       <c r="E126" s="90">
@@ -16525,7 +16515,7 @@
       <c r="C127" s="14">
         <v>500</v>
       </c>
-      <c r="D127" s="170">
+      <c r="D127" s="169">
         <v>0.75</v>
       </c>
       <c r="E127" s="90">
@@ -16602,7 +16592,7 @@
       <c r="C129" s="15">
         <v>1500</v>
       </c>
-      <c r="D129" s="170">
+      <c r="D129" s="169">
         <v>0</v>
       </c>
       <c r="J129">
@@ -16635,7 +16625,7 @@
       <c r="C130" s="14">
         <v>1000</v>
       </c>
-      <c r="D130" s="170">
+      <c r="D130" s="169">
         <v>0</v>
       </c>
       <c r="J130">
@@ -16668,7 +16658,7 @@
       <c r="C131" s="14">
         <v>1500</v>
       </c>
-      <c r="D131" s="170">
+      <c r="D131" s="169">
         <v>0</v>
       </c>
       <c r="J131">
@@ -16701,7 +16691,7 @@
       <c r="C132" s="14">
         <v>1600</v>
       </c>
-      <c r="D132" s="170">
+      <c r="D132" s="169">
         <v>0</v>
       </c>
       <c r="J132">
@@ -16734,7 +16724,7 @@
       <c r="C133" s="14">
         <v>1000</v>
       </c>
-      <c r="D133" s="170">
+      <c r="D133" s="169">
         <v>0</v>
       </c>
       <c r="J133">
@@ -16767,7 +16757,7 @@
       <c r="C134" s="105" t="s">
         <v>288</v>
       </c>
-      <c r="D134" s="170">
+      <c r="D134" s="169">
         <v>0</v>
       </c>
       <c r="J134">
@@ -16800,7 +16790,7 @@
       <c r="C135" s="14">
         <v>1100</v>
       </c>
-      <c r="D135" s="170">
+      <c r="D135" s="169">
         <v>0</v>
       </c>
       <c r="J135">
@@ -16833,7 +16823,7 @@
       <c r="C136" s="15">
         <v>920</v>
       </c>
-      <c r="D136" s="170">
+      <c r="D136" s="169">
         <v>0</v>
       </c>
       <c r="J136">
@@ -16866,7 +16856,7 @@
       <c r="C137" s="14">
         <v>1100</v>
       </c>
-      <c r="D137" s="170">
+      <c r="D137" s="169">
         <v>0</v>
       </c>
       <c r="J137">
@@ -16899,7 +16889,7 @@
       <c r="C138" s="14">
         <v>1175</v>
       </c>
-      <c r="D138" s="170">
+      <c r="D138" s="169">
         <v>0</v>
       </c>
       <c r="J138">
@@ -16932,7 +16922,7 @@
       <c r="C139" s="14">
         <v>1175</v>
       </c>
-      <c r="D139" s="170">
+      <c r="D139" s="169">
         <v>0</v>
       </c>
       <c r="J139">
@@ -16965,7 +16955,7 @@
       <c r="C140" s="14">
         <v>1200</v>
       </c>
-      <c r="D140" s="170">
+      <c r="D140" s="169">
         <v>0</v>
       </c>
       <c r="J140">
@@ -16998,7 +16988,7 @@
       <c r="C141" s="14">
         <v>1200</v>
       </c>
-      <c r="D141" s="170">
+      <c r="D141" s="169">
         <v>0</v>
       </c>
       <c r="J141">
@@ -17031,7 +17021,7 @@
       <c r="C142" s="14">
         <v>1200</v>
       </c>
-      <c r="D142" s="170">
+      <c r="D142" s="169">
         <v>0</v>
       </c>
       <c r="J142">
@@ -17064,7 +17054,7 @@
       <c r="C143" s="15">
         <v>1200</v>
       </c>
-      <c r="D143" s="170">
+      <c r="D143" s="169">
         <v>0</v>
       </c>
       <c r="J143">
@@ -17097,7 +17087,7 @@
       <c r="C144" s="14">
         <v>1180</v>
       </c>
-      <c r="D144" s="170">
+      <c r="D144" s="169">
         <v>0</v>
       </c>
       <c r="J144">
@@ -17130,7 +17120,7 @@
       <c r="C145" s="14">
         <v>1180</v>
       </c>
-      <c r="D145" s="170">
+      <c r="D145" s="169">
         <v>0</v>
       </c>
       <c r="J145">
@@ -17163,7 +17153,7 @@
       <c r="C146" s="14">
         <v>1171</v>
       </c>
-      <c r="D146" s="170">
+      <c r="D146" s="169">
         <v>0</v>
       </c>
       <c r="J146">
@@ -17196,7 +17186,7 @@
       <c r="C147" s="14">
         <v>1171</v>
       </c>
-      <c r="D147" s="170">
+      <c r="D147" s="169">
         <v>0</v>
       </c>
       <c r="J147">
@@ -17229,7 +17219,7 @@
       <c r="C148" s="14">
         <v>1100</v>
       </c>
-      <c r="D148" s="170">
+      <c r="D148" s="169">
         <v>0</v>
       </c>
       <c r="J148">
@@ -17262,7 +17252,7 @@
       <c r="C149" s="14">
         <v>1000</v>
       </c>
-      <c r="D149" s="170">
+      <c r="D149" s="169">
         <v>0</v>
       </c>
       <c r="J149">
@@ -17295,7 +17285,7 @@
       <c r="C150" s="15">
         <v>650</v>
       </c>
-      <c r="D150" s="170">
+      <c r="D150" s="169">
         <v>0</v>
       </c>
       <c r="J150">
@@ -17328,7 +17318,7 @@
       <c r="C151" s="14">
         <v>920</v>
       </c>
-      <c r="D151" s="170">
+      <c r="D151" s="169">
         <v>0</v>
       </c>
       <c r="J151">
@@ -17361,7 +17351,7 @@
       <c r="C152" s="14">
         <v>920</v>
       </c>
-      <c r="D152" s="170">
+      <c r="D152" s="169">
         <v>0</v>
       </c>
       <c r="J152">
@@ -17424,7 +17414,7 @@
       <c r="C154" s="14">
         <v>150</v>
       </c>
-      <c r="D154" s="170">
+      <c r="D154" s="169">
         <v>0.25</v>
       </c>
       <c r="E154" s="90">
@@ -17473,7 +17463,7 @@
       <c r="C155" s="14">
         <v>100</v>
       </c>
-      <c r="D155" s="170">
+      <c r="D155" s="169">
         <v>0.25</v>
       </c>
       <c r="E155" s="90">
@@ -17522,7 +17512,7 @@
       <c r="C156" s="14">
         <v>100</v>
       </c>
-      <c r="D156" s="170">
+      <c r="D156" s="169">
         <v>0.25</v>
       </c>
       <c r="E156" s="90">
@@ -17571,7 +17561,7 @@
       <c r="C157" s="15">
         <v>30</v>
       </c>
-      <c r="D157" s="170">
+      <c r="D157" s="169">
         <v>0.25</v>
       </c>
       <c r="E157" s="90">
@@ -17620,7 +17610,7 @@
       <c r="C158" s="14">
         <v>30</v>
       </c>
-      <c r="D158" s="170">
+      <c r="D158" s="169">
         <v>0.25</v>
       </c>
       <c r="E158" s="90">
@@ -17669,7 +17659,7 @@
       <c r="C159" s="14">
         <v>30</v>
       </c>
-      <c r="D159" s="170">
+      <c r="D159" s="169">
         <v>0.25</v>
       </c>
       <c r="E159" s="90">
@@ -17718,7 +17708,7 @@
       <c r="C160" s="14">
         <v>30</v>
       </c>
-      <c r="D160" s="170">
+      <c r="D160" s="169">
         <v>0.25</v>
       </c>
       <c r="E160" s="90">
@@ -17767,7 +17757,7 @@
       <c r="C161" s="14">
         <v>60</v>
       </c>
-      <c r="D161" s="170">
+      <c r="D161" s="169">
         <v>0.25</v>
       </c>
       <c r="E161" s="90">
@@ -17816,7 +17806,7 @@
       <c r="C162" s="14">
         <v>60</v>
       </c>
-      <c r="D162" s="170">
+      <c r="D162" s="169">
         <v>0.25</v>
       </c>
       <c r="E162" s="90">
@@ -17865,7 +17855,7 @@
       <c r="C163" s="14">
         <v>120</v>
       </c>
-      <c r="D163" s="170">
+      <c r="D163" s="169">
         <v>0.25</v>
       </c>
       <c r="E163" s="90">
@@ -17914,7 +17904,7 @@
       <c r="C164" s="15">
         <v>40</v>
       </c>
-      <c r="D164" s="170">
+      <c r="D164" s="169">
         <v>0</v>
       </c>
       <c r="E164" s="90">
@@ -17963,7 +17953,7 @@
       <c r="C165" s="14">
         <v>23</v>
       </c>
-      <c r="D165" s="170">
+      <c r="D165" s="169">
         <v>0</v>
       </c>
       <c r="E165" s="90">
@@ -18002,52 +17992,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:15" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="167">
+    <row r="166" spans="1:15" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="162">
         <v>10.005000000000001</v>
       </c>
-      <c r="B166" s="168" t="s">
+      <c r="B166" s="163" t="s">
         <v>199</v>
       </c>
-      <c r="C166" s="169">
+      <c r="C166" s="164">
         <v>33</v>
       </c>
-      <c r="D166" s="170">
+      <c r="D166" s="169">
         <v>0.25</v>
       </c>
-      <c r="E166" s="174">
+      <c r="E166" s="167">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F166" s="170">
+      <c r="F166" s="165">
         <f t="shared" si="5"/>
         <v>0.72</v>
       </c>
-      <c r="G166" s="170">
-        <v>1</v>
-      </c>
-      <c r="H166" s="170">
-        <v>0</v>
-      </c>
-      <c r="I166" s="170">
-        <v>0</v>
-      </c>
-      <c r="J166" s="170">
-        <v>0</v>
-      </c>
-      <c r="K166" s="170">
-        <v>1</v>
-      </c>
-      <c r="L166" s="170">
-        <v>1</v>
-      </c>
-      <c r="M166" s="170">
-        <v>0</v>
-      </c>
-      <c r="N166" s="170">
+      <c r="G166" s="165">
+        <v>1</v>
+      </c>
+      <c r="H166" s="165">
+        <v>0</v>
+      </c>
+      <c r="I166" s="165">
+        <v>0</v>
+      </c>
+      <c r="J166" s="165">
+        <v>0</v>
+      </c>
+      <c r="K166" s="165">
+        <v>1</v>
+      </c>
+      <c r="L166" s="165">
+        <v>1</v>
+      </c>
+      <c r="M166" s="165">
+        <v>0</v>
+      </c>
+      <c r="N166" s="165">
         <f t="shared" si="4"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="O166" s="170">
+      <c r="O166" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -18061,7 +18051,7 @@
       <c r="C167" s="14">
         <v>30</v>
       </c>
-      <c r="D167" s="170">
+      <c r="D167" s="169">
         <v>0</v>
       </c>
       <c r="E167" s="90">
@@ -18110,7 +18100,7 @@
       <c r="C168" s="14">
         <v>133</v>
       </c>
-      <c r="D168" s="170">
+      <c r="D168" s="169">
         <v>0.25</v>
       </c>
       <c r="E168" s="90">
@@ -18159,7 +18149,7 @@
       <c r="C169" s="14">
         <v>138</v>
       </c>
-      <c r="D169" s="170">
+      <c r="D169" s="169">
         <v>0.25</v>
       </c>
       <c r="E169" s="90">
@@ -18208,7 +18198,7 @@
       <c r="C170" s="14">
         <v>138</v>
       </c>
-      <c r="D170" s="170">
+      <c r="D170" s="169">
         <v>0.25</v>
       </c>
       <c r="E170" s="90">
@@ -18257,7 +18247,7 @@
       <c r="C171" s="15">
         <v>96</v>
       </c>
-      <c r="D171" s="170">
+      <c r="D171" s="169">
         <v>0.25</v>
       </c>
       <c r="E171" s="90">
@@ -18306,7 +18296,7 @@
       <c r="C172" s="14">
         <v>96</v>
       </c>
-      <c r="D172" s="170">
+      <c r="D172" s="169">
         <v>0.25</v>
       </c>
       <c r="E172" s="90">
@@ -18355,7 +18345,7 @@
       <c r="C173" s="14">
         <v>215</v>
       </c>
-      <c r="D173" s="170">
+      <c r="D173" s="169">
         <v>0.25</v>
       </c>
       <c r="E173" s="90">
@@ -18404,7 +18394,7 @@
       <c r="C174" s="14">
         <v>147.5</v>
       </c>
-      <c r="D174" s="170">
+      <c r="D174" s="169">
         <v>0.25</v>
       </c>
       <c r="E174" s="90">
@@ -18453,7 +18443,7 @@
       <c r="C175" s="14">
         <v>140</v>
       </c>
-      <c r="D175" s="170">
+      <c r="D175" s="169">
         <v>0.25</v>
       </c>
       <c r="E175" s="90">
@@ -18502,7 +18492,7 @@
       <c r="C176" s="14">
         <v>48</v>
       </c>
-      <c r="D176" s="170">
+      <c r="D176" s="169">
         <v>0.25</v>
       </c>
       <c r="E176" s="90">
@@ -18551,7 +18541,7 @@
       <c r="C177" s="14">
         <v>48</v>
       </c>
-      <c r="D177" s="170">
+      <c r="D177" s="169">
         <v>0.25</v>
       </c>
       <c r="E177" s="90">
@@ -18630,7 +18620,7 @@
       <c r="C179" s="14">
         <v>4.55</v>
       </c>
-      <c r="D179" s="170">
+      <c r="D179" s="169">
         <v>0</v>
       </c>
       <c r="E179" s="90">
@@ -18678,7 +18668,7 @@
       <c r="C180" s="14">
         <v>3.6</v>
       </c>
-      <c r="D180" s="170">
+      <c r="D180" s="169">
         <v>0</v>
       </c>
       <c r="J180">
@@ -18711,7 +18701,7 @@
       <c r="C181" s="14">
         <v>8.25</v>
       </c>
-      <c r="D181" s="170">
+      <c r="D181" s="169">
         <v>0</v>
       </c>
       <c r="J181">
@@ -18744,7 +18734,7 @@
       <c r="C182" s="14">
         <v>63.3</v>
       </c>
-      <c r="D182" s="170">
+      <c r="D182" s="169">
         <v>0</v>
       </c>
       <c r="J182">
@@ -18777,7 +18767,7 @@
       <c r="C183" s="14">
         <v>57.8</v>
       </c>
-      <c r="D183" s="170">
+      <c r="D183" s="169">
         <v>0</v>
       </c>
       <c r="J183">
@@ -18810,7 +18800,7 @@
       <c r="C184" s="14">
         <v>73.5</v>
       </c>
-      <c r="D184" s="170">
+      <c r="D184" s="169">
         <v>0</v>
       </c>
       <c r="J184">
@@ -18843,7 +18833,7 @@
       <c r="C185" s="15">
         <v>3.36</v>
       </c>
-      <c r="D185" s="170">
+      <c r="D185" s="169">
         <v>0</v>
       </c>
       <c r="J185">
@@ -18876,7 +18866,7 @@
       <c r="C186" s="14">
         <v>18</v>
       </c>
-      <c r="D186" s="170">
+      <c r="D186" s="169">
         <v>0</v>
       </c>
       <c r="J186">
@@ -18909,7 +18899,7 @@
       <c r="C187" s="14">
         <v>7.8</v>
       </c>
-      <c r="D187" s="170">
+      <c r="D187" s="169">
         <v>0</v>
       </c>
       <c r="J187">
@@ -18942,7 +18932,7 @@
       <c r="C188" s="14">
         <v>2.7</v>
       </c>
-      <c r="D188" s="170">
+      <c r="D188" s="169">
         <v>0</v>
       </c>
       <c r="J188">
@@ -18975,7 +18965,7 @@
       <c r="C189" s="14">
         <v>2.7</v>
       </c>
-      <c r="D189" s="170">
+      <c r="D189" s="169">
         <v>0</v>
       </c>
       <c r="J189">
@@ -19008,7 +18998,7 @@
       <c r="C190" s="14">
         <v>21.5</v>
       </c>
-      <c r="D190" s="170">
+      <c r="D190" s="169">
         <v>0</v>
       </c>
       <c r="J190">
@@ -19041,7 +19031,7 @@
       <c r="C191" s="14">
         <v>8.5</v>
       </c>
-      <c r="D191" s="170">
+      <c r="D191" s="169">
         <v>0.25</v>
       </c>
       <c r="E191" s="90">
@@ -19090,7 +19080,7 @@
       <c r="C192" s="15">
         <v>2.9</v>
       </c>
-      <c r="D192" s="170">
+      <c r="D192" s="169">
         <v>0</v>
       </c>
       <c r="J192">
@@ -19123,7 +19113,7 @@
       <c r="C193" s="14">
         <v>40.5</v>
       </c>
-      <c r="D193" s="170">
+      <c r="D193" s="169">
         <v>0.25</v>
       </c>
       <c r="E193" s="90">
@@ -19172,7 +19162,7 @@
       <c r="C194" s="14">
         <v>40.5</v>
       </c>
-      <c r="D194" s="170">
+      <c r="D194" s="169">
         <v>0.25</v>
       </c>
       <c r="E194" s="90">
@@ -19221,7 +19211,7 @@
       <c r="C195" s="14">
         <v>40.5</v>
       </c>
-      <c r="D195" s="170">
+      <c r="D195" s="169">
         <v>0.25</v>
       </c>
       <c r="E195" s="90">
@@ -19270,7 +19260,7 @@
       <c r="C196" s="14">
         <v>40.5</v>
       </c>
-      <c r="D196" s="170">
+      <c r="D196" s="169">
         <v>0.25</v>
       </c>
       <c r="E196" s="90">
@@ -19319,7 +19309,7 @@
       <c r="C197" s="14">
         <v>40.5</v>
       </c>
-      <c r="D197" s="170">
+      <c r="D197" s="169">
         <v>0.25</v>
       </c>
       <c r="E197" s="90">
@@ -19368,7 +19358,7 @@
       <c r="C198" s="14">
         <v>40.5</v>
       </c>
-      <c r="D198" s="170">
+      <c r="D198" s="169">
         <v>0.25</v>
       </c>
       <c r="E198" s="90">
@@ -19417,7 +19407,7 @@
       <c r="C199" s="15">
         <v>6.1</v>
       </c>
-      <c r="D199" s="170">
+      <c r="D199" s="169">
         <v>0.25</v>
       </c>
       <c r="E199" s="90">
@@ -19466,7 +19456,7 @@
       <c r="C200" s="14">
         <v>7.9</v>
       </c>
-      <c r="D200" s="170">
+      <c r="D200" s="169">
         <v>0.25</v>
       </c>
       <c r="E200" s="90">
@@ -19515,7 +19505,7 @@
       <c r="C201" s="14">
         <v>5.6</v>
       </c>
-      <c r="D201" s="170">
+      <c r="D201" s="169">
         <v>0.25</v>
       </c>
       <c r="E201" s="90">
@@ -19564,7 +19554,7 @@
       <c r="C202" s="14">
         <v>3.1</v>
       </c>
-      <c r="D202" s="170">
+      <c r="D202" s="169">
         <v>0</v>
       </c>
       <c r="J202">
@@ -19597,7 +19587,7 @@
       <c r="C203" s="14">
         <v>22</v>
       </c>
-      <c r="D203" s="170">
+      <c r="D203" s="169">
         <v>0</v>
       </c>
       <c r="J203">
@@ -19630,7 +19620,7 @@
       <c r="C204" s="14">
         <v>3.4</v>
       </c>
-      <c r="D204" s="170">
+      <c r="D204" s="169">
         <v>0</v>
       </c>
       <c r="J204">
@@ -19663,7 +19653,7 @@
       <c r="C205" s="14">
         <v>2.1</v>
       </c>
-      <c r="D205" s="170">
+      <c r="D205" s="169">
         <v>0</v>
       </c>
       <c r="J205">
@@ -19696,7 +19686,7 @@
       <c r="C206" s="15">
         <v>1.3</v>
       </c>
-      <c r="D206" s="170">
+      <c r="D206" s="169">
         <v>0</v>
       </c>
       <c r="J206">
@@ -19729,7 +19719,7 @@
       <c r="C207" s="14">
         <v>2.7</v>
       </c>
-      <c r="D207" s="170">
+      <c r="D207" s="169">
         <v>0</v>
       </c>
       <c r="J207">
@@ -19762,7 +19752,7 @@
       <c r="C208" s="14">
         <v>95</v>
       </c>
-      <c r="D208" s="170">
+      <c r="D208" s="169">
         <v>0</v>
       </c>
       <c r="J208">
@@ -19795,7 +19785,7 @@
       <c r="C209" s="105" t="s">
         <v>287</v>
       </c>
-      <c r="D209" s="170">
+      <c r="D209" s="169">
         <v>0</v>
       </c>
       <c r="J209">
@@ -19828,7 +19818,7 @@
       <c r="C210" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D210" s="170">
+      <c r="D210" s="169">
         <v>0.25</v>
       </c>
       <c r="E210" s="90">
@@ -19877,7 +19867,7 @@
       <c r="C211" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D211" s="170">
+      <c r="D211" s="169">
         <v>0.25</v>
       </c>
       <c r="E211" s="90">
@@ -19916,52 +19906,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:15" s="170" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="175">
+    <row r="212" spans="1:15" s="165" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A212" s="168">
         <v>12.003</v>
       </c>
-      <c r="B212" s="168" t="s">
+      <c r="B212" s="163" t="s">
         <v>247</v>
       </c>
-      <c r="C212" s="169" t="s">
+      <c r="C212" s="164" t="s">
         <v>287</v>
       </c>
-      <c r="D212" s="170">
+      <c r="D212" s="169">
         <v>0.25</v>
       </c>
-      <c r="E212" s="174">
+      <c r="E212" s="167">
         <v>0.1</v>
       </c>
-      <c r="F212" s="170">
+      <c r="F212" s="165">
         <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
-      <c r="G212" s="170">
-        <v>1</v>
-      </c>
-      <c r="H212" s="170">
-        <v>0</v>
-      </c>
-      <c r="I212" s="170">
-        <v>0</v>
-      </c>
-      <c r="J212" s="170">
-        <v>0</v>
-      </c>
-      <c r="K212" s="170">
-        <v>1</v>
-      </c>
-      <c r="L212" s="170">
-        <v>1</v>
-      </c>
-      <c r="M212" s="170">
-        <v>0</v>
-      </c>
-      <c r="N212" s="170">
+      <c r="G212" s="165">
+        <v>1</v>
+      </c>
+      <c r="H212" s="165">
+        <v>0</v>
+      </c>
+      <c r="I212" s="165">
+        <v>0</v>
+      </c>
+      <c r="J212" s="165">
+        <v>0</v>
+      </c>
+      <c r="K212" s="165">
+        <v>1</v>
+      </c>
+      <c r="L212" s="165">
+        <v>1</v>
+      </c>
+      <c r="M212" s="165">
+        <v>0</v>
+      </c>
+      <c r="N212" s="165">
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
-      <c r="O212" s="170">
+      <c r="O212" s="165">
         <v>0.8</v>
       </c>
     </row>
@@ -19975,7 +19965,7 @@
       <c r="C213" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="D213" s="170">
+      <c r="D213" s="169">
         <v>0.25</v>
       </c>
       <c r="E213" s="90">
@@ -20024,7 +20014,7 @@
       <c r="C214" s="105" t="s">
         <v>289</v>
       </c>
-      <c r="D214" s="170">
+      <c r="D214" s="169">
         <v>0</v>
       </c>
       <c r="L214">
@@ -20051,7 +20041,7 @@
       <c r="C215" s="14">
         <v>0.3</v>
       </c>
-      <c r="D215" s="170">
+      <c r="D215" s="169">
         <v>0</v>
       </c>
       <c r="L215">
@@ -20078,7 +20068,7 @@
       <c r="C216" s="14">
         <v>0.3</v>
       </c>
-      <c r="D216" s="170">
+      <c r="D216" s="169">
         <v>0</v>
       </c>
       <c r="L216">
@@ -20105,7 +20095,7 @@
       <c r="C217" s="14">
         <v>0.25</v>
       </c>
-      <c r="D217" s="170">
+      <c r="D217" s="169">
         <v>0</v>
       </c>
       <c r="L217">
@@ -20132,7 +20122,7 @@
       <c r="C218" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D218" s="170">
+      <c r="D218" s="169">
         <v>0</v>
       </c>
       <c r="L218">
@@ -20159,7 +20149,7 @@
       <c r="C219" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D219" s="170">
+      <c r="D219" s="169">
         <v>0</v>
       </c>
       <c r="L219">
@@ -20186,7 +20176,7 @@
       <c r="C220" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="D220" s="170">
+      <c r="D220" s="169">
         <v>0</v>
       </c>
       <c r="L220">
@@ -20213,7 +20203,7 @@
       <c r="C221" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D221" s="170">
+      <c r="D221" s="169">
         <v>0</v>
       </c>
       <c r="L221">
@@ -20240,7 +20230,7 @@
       <c r="C222" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D222" s="170">
+      <c r="D222" s="169">
         <v>0</v>
       </c>
       <c r="L222">
@@ -20267,7 +20257,7 @@
       <c r="C223" s="105" t="s">
         <v>288</v>
       </c>
-      <c r="D223" s="170">
+      <c r="D223" s="169">
         <v>0</v>
       </c>
       <c r="L223">
@@ -20294,7 +20284,7 @@
       <c r="C224" s="14">
         <v>1180</v>
       </c>
-      <c r="D224" s="170">
+      <c r="D224" s="169">
         <v>0</v>
       </c>
       <c r="L224">
@@ -20321,7 +20311,7 @@
       <c r="C225" s="14">
         <v>1360</v>
       </c>
-      <c r="D225" s="170">
+      <c r="D225" s="169">
         <v>0</v>
       </c>
       <c r="L225">
@@ -20348,7 +20338,7 @@
       <c r="C226" s="14">
         <v>1200</v>
       </c>
-      <c r="D226" s="170">
+      <c r="D226" s="169">
         <v>0</v>
       </c>
       <c r="L226">
@@ -20375,7 +20365,7 @@
       <c r="C227" s="15">
         <v>1500</v>
       </c>
-      <c r="D227" s="170">
+      <c r="D227" s="169">
         <v>0</v>
       </c>
       <c r="L227">
@@ -20402,7 +20392,7 @@
       <c r="C228" s="14">
         <v>1050</v>
       </c>
-      <c r="D228" s="170">
+      <c r="D228" s="169">
         <v>0</v>
       </c>
       <c r="L228">
@@ -20427,16 +20417,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85F04A2-D279-47E1-9F8D-60F5321B6646}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="60.26953125" customWidth="1"/>
-    <col min="2" max="20" width="20.6328125" customWidth="1"/>
+    <col min="2" max="6" width="20.6328125" customWidth="1"/>
+    <col min="7" max="8" width="20.6328125" style="116" customWidth="1"/>
+    <col min="9" max="12" width="20.6328125" customWidth="1"/>
+    <col min="13" max="13" width="20.6328125" style="116" customWidth="1"/>
+    <col min="14" max="16" width="20.6328125" customWidth="1"/>
+    <col min="17" max="17" width="20.6328125" style="116" customWidth="1"/>
+    <col min="18" max="20" width="20.6328125" customWidth="1"/>
     <col min="21" max="21" width="10.90625" style="90"/>
   </cols>
   <sheetData>
@@ -20457,10 +20453,10 @@
         <v>317</v>
       </c>
       <c r="F1" s="100"/>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="176" t="s">
         <v>319</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="176" t="s">
         <v>338</v>
       </c>
       <c r="I1" s="100"/>
@@ -20471,7 +20467,7 @@
       <c r="L1" s="99" t="s">
         <v>340</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="M1" s="176" t="s">
         <v>342</v>
       </c>
       <c r="N1" s="100" t="s">
@@ -20481,7 +20477,7 @@
         <v>296</v>
       </c>
       <c r="P1" s="99"/>
-      <c r="Q1" s="99" t="s">
+      <c r="Q1" s="176" t="s">
         <v>346</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -20510,10 +20506,10 @@
       <c r="F2" s="93" t="s">
         <v>299</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="177" t="s">
         <v>343</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="177" t="s">
         <v>328</v>
       </c>
       <c r="I2" s="93" t="s">
@@ -20528,7 +20524,7 @@
       <c r="L2" s="92" t="s">
         <v>301</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="177" t="s">
         <v>343</v>
       </c>
       <c r="N2" s="92" t="s">
@@ -20540,7 +20536,7 @@
       <c r="P2" s="93" t="s">
         <v>299</v>
       </c>
-      <c r="Q2" s="92" t="s">
+      <c r="Q2" s="177" t="s">
         <v>344</v>
       </c>
       <c r="R2" s="93" t="s">
@@ -20554,7 +20550,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="156">
+      <c r="A3" s="151">
         <v>2</v>
       </c>
       <c r="B3" s="109" t="s">
@@ -20573,11 +20569,11 @@
       <c r="F3" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G3" s="101">
+      <c r="G3" s="178">
         <f>D3*E3</f>
         <v>102</v>
       </c>
-      <c r="H3" s="101">
+      <c r="H3" s="178">
         <f>C3*J3</f>
         <v>66</v>
       </c>
@@ -20594,7 +20590,7 @@
         <f>18*C3</f>
         <v>21.599999999999998</v>
       </c>
-      <c r="M3" s="95"/>
+      <c r="M3" s="178"/>
       <c r="N3" s="94">
         <v>-25</v>
       </c>
@@ -20604,7 +20600,7 @@
       <c r="P3" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q3" s="94">
+      <c r="Q3" s="178">
         <f>R3*85</f>
         <v>42.5</v>
       </c>
@@ -20620,7 +20616,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="156">
+      <c r="A4" s="151">
         <v>1</v>
       </c>
       <c r="B4" s="109" t="s">
@@ -20638,11 +20634,11 @@
       <c r="F4" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G4" s="101">
+      <c r="G4" s="178">
         <f t="shared" ref="G4:G14" si="0">D4*E4</f>
         <v>340</v>
       </c>
-      <c r="H4" s="101">
+      <c r="H4" s="178">
         <f>C4*J4</f>
         <v>75</v>
       </c>
@@ -20659,7 +20655,7 @@
         <f>18*C4</f>
         <v>45</v>
       </c>
-      <c r="M4" s="95"/>
+      <c r="M4" s="178"/>
       <c r="N4" s="94">
         <v>-25</v>
       </c>
@@ -20669,7 +20665,7 @@
       <c r="P4" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q4" s="94">
+      <c r="Q4" s="178">
         <f t="shared" ref="Q4:Q14" si="1">R4*85</f>
         <v>425</v>
       </c>
@@ -20685,10 +20681,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="156" t="s">
+      <c r="A5" s="151" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="109" t="s">
         <v>306</v>
       </c>
       <c r="C5" s="93">
@@ -20703,11 +20699,11 @@
       <c r="F5" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G5" s="101">
+      <c r="G5" s="178">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H5" s="101">
+      <c r="H5" s="178">
         <f>C5*J5*0.036</f>
         <v>4.9499999999999993</v>
       </c>
@@ -20724,7 +20720,7 @@
         <f>C5*15</f>
         <v>37.5</v>
       </c>
-      <c r="M5" s="95"/>
+      <c r="M5" s="178"/>
       <c r="N5" s="94"/>
       <c r="O5" s="94">
         <v>0</v>
@@ -20732,7 +20728,7 @@
       <c r="P5" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q5" s="94">
+      <c r="Q5" s="178">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -20748,10 +20744,10 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="151" t="s">
         <v>324</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="109" t="s">
         <v>307</v>
       </c>
       <c r="C6" s="93">
@@ -20766,11 +20762,11 @@
       <c r="F6" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G6" s="101">
+      <c r="G6" s="178">
         <f t="shared" si="0"/>
         <v>25.5</v>
       </c>
-      <c r="H6" s="101">
+      <c r="H6" s="178">
         <f>C6*J6*0.1</f>
         <v>4.6749999999999998</v>
       </c>
@@ -20787,7 +20783,7 @@
         <f t="shared" ref="L6:L14" si="2">C6*15</f>
         <v>12.75</v>
       </c>
-      <c r="M6" s="95"/>
+      <c r="M6" s="178"/>
       <c r="N6" s="94"/>
       <c r="O6" s="94">
         <v>0</v>
@@ -20795,7 +20791,7 @@
       <c r="P6" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q6" s="94">
+      <c r="Q6" s="178">
         <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
@@ -20811,10 +20807,10 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="156">
+      <c r="A7" s="151">
         <v>10</v>
       </c>
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="109" t="s">
         <v>308</v>
       </c>
       <c r="C7" s="93">
@@ -20829,11 +20825,11 @@
       <c r="F7" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="178">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H7" s="101">
+      <c r="H7" s="178">
         <f>C7*J7*0.2</f>
         <v>28.8</v>
       </c>
@@ -20850,7 +20846,7 @@
         <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
-      <c r="M7" s="95"/>
+      <c r="M7" s="178"/>
       <c r="N7" s="94"/>
       <c r="O7" s="94">
         <v>0</v>
@@ -20858,7 +20854,7 @@
       <c r="P7" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q7" s="94">
+      <c r="Q7" s="178">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
@@ -20874,10 +20870,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="156" t="s">
+      <c r="A8" s="151" t="s">
         <v>322</v>
       </c>
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="109" t="s">
         <v>309</v>
       </c>
       <c r="C8" s="93">
@@ -20893,11 +20889,11 @@
       <c r="F8" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G8" s="101">
+      <c r="G8" s="178">
         <f t="shared" si="0"/>
         <v>2269.5000000000005</v>
       </c>
-      <c r="H8" s="101">
+      <c r="H8" s="178">
         <f>C8*J8</f>
         <v>0</v>
       </c>
@@ -20914,7 +20910,7 @@
         <f t="shared" si="2"/>
         <v>122.99999999999999</v>
       </c>
-      <c r="M8" s="95"/>
+      <c r="M8" s="178"/>
       <c r="N8" s="94">
         <v>-165</v>
       </c>
@@ -20924,7 +20920,7 @@
       <c r="P8" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q8" s="94">
+      <c r="Q8" s="178">
         <f t="shared" si="1"/>
         <v>2787.9999999999995</v>
       </c>
@@ -20941,10 +20937,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="151" t="s">
         <v>320</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="109" t="s">
         <v>311</v>
       </c>
       <c r="C9" s="93">
@@ -20960,11 +20956,11 @@
       <c r="F9" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G9" s="101">
+      <c r="G9" s="178">
         <f t="shared" si="0"/>
         <v>685.95</v>
       </c>
-      <c r="H9" s="101">
+      <c r="H9" s="178">
         <f>C9*J9</f>
         <v>0</v>
       </c>
@@ -20981,7 +20977,7 @@
         <f t="shared" si="2"/>
         <v>40.35</v>
       </c>
-      <c r="M9" s="95"/>
+      <c r="M9" s="178"/>
       <c r="N9" s="94">
         <v>-125</v>
       </c>
@@ -20991,7 +20987,7 @@
       <c r="P9" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q9" s="94">
+      <c r="Q9" s="178">
         <f t="shared" si="1"/>
         <v>914.6</v>
       </c>
@@ -21008,10 +21004,10 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="156" t="s">
+      <c r="A10" s="151" t="s">
         <v>321</v>
       </c>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="109" t="s">
         <v>312</v>
       </c>
       <c r="C10" s="93">
@@ -21027,11 +21023,11 @@
       <c r="F10" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G10" s="101">
+      <c r="G10" s="178">
         <f t="shared" si="0"/>
         <v>2001.7499999999998</v>
       </c>
-      <c r="H10" s="101">
+      <c r="H10" s="178">
         <f>C10*J10</f>
         <v>0</v>
       </c>
@@ -21048,7 +21044,7 @@
         <f t="shared" si="2"/>
         <v>117.75</v>
       </c>
-      <c r="M10" s="95"/>
+      <c r="M10" s="178"/>
       <c r="N10" s="94">
         <v>-165</v>
       </c>
@@ -21058,7 +21054,7 @@
       <c r="P10" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q10" s="94">
+      <c r="Q10" s="178">
         <f t="shared" si="1"/>
         <v>2669</v>
       </c>
@@ -21075,10 +21071,10 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="156">
+      <c r="A11" s="151">
         <v>7</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="109" t="s">
         <v>313</v>
       </c>
       <c r="C11" s="93">
@@ -21093,11 +21089,11 @@
       <c r="F11" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="101">
+      <c r="G11" s="178">
         <f t="shared" si="0"/>
         <v>127.5</v>
       </c>
-      <c r="H11" s="101">
+      <c r="H11" s="178">
         <f>C11*J11</f>
         <v>29.4</v>
       </c>
@@ -21114,7 +21110,7 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="M11" s="95"/>
+      <c r="M11" s="178"/>
       <c r="N11" s="94">
         <v>-5</v>
       </c>
@@ -21124,7 +21120,7 @@
       <c r="P11" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q11" s="94">
+      <c r="Q11" s="178">
         <f t="shared" si="1"/>
         <v>144.5</v>
       </c>
@@ -21140,10 +21136,10 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="156">
+      <c r="A12" s="151">
         <v>9.0039999999999996</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="109" t="s">
         <v>314</v>
       </c>
       <c r="C12" s="93">
@@ -21158,11 +21154,11 @@
       <c r="F12" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G12" s="101">
+      <c r="G12" s="178">
         <f>D12*E12</f>
         <v>51</v>
       </c>
-      <c r="H12" s="101">
+      <c r="H12" s="178">
         <f>C12*J12*0.1</f>
         <v>17.600000000000001</v>
       </c>
@@ -21179,7 +21175,7 @@
         <f t="shared" si="2"/>
         <v>16.5</v>
       </c>
-      <c r="M12" s="95"/>
+      <c r="M12" s="178"/>
       <c r="N12" s="94">
         <v>-10</v>
       </c>
@@ -21189,7 +21185,7 @@
       <c r="P12" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q12" s="94">
+      <c r="Q12" s="178">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
@@ -21205,10 +21201,10 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="156">
+      <c r="A13" s="151">
         <v>5</v>
       </c>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="109" t="s">
         <v>315</v>
       </c>
       <c r="C13" s="93">
@@ -21223,11 +21219,11 @@
       <c r="F13" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="178">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H13" s="101">
+      <c r="H13" s="178">
         <f>C13*J13*0.1</f>
         <v>32.300000000000004</v>
       </c>
@@ -21244,7 +21240,7 @@
         <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
-      <c r="M13" s="95"/>
+      <c r="M13" s="178"/>
       <c r="N13" s="94"/>
       <c r="O13" s="94">
         <v>0</v>
@@ -21252,7 +21248,7 @@
       <c r="P13" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q13" s="94">
+      <c r="Q13" s="178">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
@@ -21268,10 +21264,10 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="156">
+      <c r="A14" s="151">
         <v>12</v>
       </c>
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="109" t="s">
         <v>316</v>
       </c>
       <c r="C14" s="93">
@@ -21286,11 +21282,11 @@
       <c r="F14" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="G14" s="101">
+      <c r="G14" s="178">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H14" s="101">
+      <c r="H14" s="178">
         <f>C14*J14*0.2</f>
         <v>25.2</v>
       </c>
@@ -21307,7 +21303,7 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="M14" s="95"/>
+      <c r="M14" s="178"/>
       <c r="N14" s="94"/>
       <c r="O14" s="94">
         <v>0</v>
@@ -21315,7 +21311,7 @@
       <c r="P14" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="Q14" s="94">
+      <c r="Q14" s="178">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
@@ -21328,6 +21324,11 @@
       <c r="T14" s="96"/>
       <c r="U14" s="90">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="116" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -21341,7 +21342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92076F68-4096-4278-8AE0-53638196C0AA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>